<commit_message>
Add cargar_estructura method to Estructura class
Introduces a new method cargar_estructura in the Estructura class to streamline the process of adding nodes, bars, and loads. Updates main.py to use this new method, improving code organization and clarity. Also updates the Datos_template.xlsx file.
</commit_message>
<xml_diff>
--- a/data/Datos_template.xlsx
+++ b/data/Datos_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Nodo"/>
@@ -725,7 +725,7 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9" t="s">
@@ -1705,7 +1705,7 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>